<commit_message>
adde express js question and tab view
</commit_message>
<xml_diff>
--- a/Mearn Interview Question.xlsx
+++ b/Mearn Interview Question.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="JavaScript Core and Advance" sheetId="1" r:id="rId1"/>
     <sheet name="Node JS Core and Advance" sheetId="2" r:id="rId2"/>
     <sheet name="React JS Core and Advance" sheetId="3" r:id="rId3"/>
-    <sheet name="Mongo DB Core and Advance" sheetId="4" r:id="rId4"/>
-    <sheet name="Technical Interview Question" sheetId="5" r:id="rId5"/>
+    <sheet name="Express Js Interview Question" sheetId="6" r:id="rId4"/>
+    <sheet name="Mongo DB Core and Advance" sheetId="4" r:id="rId5"/>
+    <sheet name="Technical Interview Question" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -2215,6 +2216,257 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+1. What is Express.js, and how does it differ from Node.js?
+Express.js is a web application framework built on top of Node.js, designed to simplify the process of building web applications and APIs. It provides a robust set of features for web and mobile applications, such as routing, middleware support, and a simpler way to handle HTTP requests.
+Differences between Express.js and Node.js:
+Framework vs. Runtime: Node.js is a runtime environment that allows JavaScript to run on the server side, while Express.js is a framework built on Node.js to facilitate web application development.
+Features: Express provides features like routing, middleware, and template rendering that simplify server-side programming, whereas Node.js provides core functionalities for building server applications.
+2. How do you set up a basic Express server?
+To set up a basic Express server:
+Install Express using npm:
+bash
+Copy code
+npm install express
+Create a server file, e.g., server.js, and set up the server:
+javascript
+Copy code
+const express = require('express');
+const app = express();
+const PORT = process.env.PORT || 3000;
+app.get('/', (req, res) =&gt; {
+  res.send('Hello World!');
+});
+app.listen(PORT, () =&gt; {
+  console.log(`Server is running on http://localhost:${PORT}`);
+});
+Run the server with:
+bash
+Copy code
+node server.js
+3. What are middleware in Express, and how do they work?
+Middleware in Express are functions that execute during the request-response cycle. They have access to the request and response objects and can modify them, end the request-response cycle, or call the next middleware function in the stack.
+How Middleware Works:
+Middleware functions can perform tasks such as logging, authentication, body parsing, and error handling.
+They are defined using app.use() or as route-specific middleware.
+Middleware functions can be called in sequence by using the next() function to pass control to the next function.
+4. How can you handle routing in Express?
+Routing in Express is handled using methods that correspond to HTTP verbs. You define routes using the following syntax:
+javascript
+Copy code
+app.get('/path', (req, res) =&gt; {
+  // Handle GET request
+});
+app.post('/path', (req, res) =&gt; {
+  // Handle POST request
+});
+// Other HTTP methods: put, delete, etc.
+You can also define route parameters and query parameters:
+javascript
+Copy code
+app.get('/user/:id', (req, res) =&gt; {
+  const userId = req.params.id;
+  res.send(`User ID: ${userId}`);
+});
+5. How do you handle errors in an Express application?
+Error handling in Express is done through middleware. You can define an error-handling middleware function that takes four arguments: err, req, res, and next.
+javascript
+Copy code
+app.use((err, req, res, next) =&gt; {
+  console.error(err.stack);
+  res.status(500).send('Something broke!');
+});
+This middleware should be defined after all other middleware and routes, ensuring it catches errors from earlier processes.
+6. What are the different types of HTTP methods supported by Express?
+Express supports the following HTTP methods:
+GET: Retrieve data from the server.
+POST: Send data to the server (e.g., create a resource).
+PUT: Update existing resources.
+DELETE: Remove resources.
+PATCH: Partially update a resource.
+OPTIONS: Describe the communication options for the target resource.
+7. How can you serve static files using Express?
+You can serve static files using the built-in express.static middleware:
+javascript
+Copy code
+const path = require('path');
+app.use(express.static(path.join(__dirname, 'public')));
+In this example, all files in the public directory will be served as static files.
+8. How do you parse JSON and URL-encoded data in Express?
+To parse JSON and URL-encoded data, use the following middleware:
+For JSON data:
+javascript
+Copy code
+app.use(express.json());
+For URL-encoded data (form submissions):
+javascript
+Copy code
+app.use(express.urlencoded({ extended: true }));
+9. What is the purpose of the app.use() function?
+The app.use() function in Express is used to mount middleware functions at a specified path. It can be used to apply middleware globally or to specific routes. For example:
+javascript
+Copy code
+app.use(express.json()); // Apply JSON parsing middleware globally
+app.use('/api', apiRouter); // Apply apiRouter middleware to /api routes
+10. How can you implement CORS in an Express application?
+CORS (Cross-Origin Resource Sharing) can be implemented using the cors middleware package:
+Install the CORS package:
+bash
+Copy code
+npm install cors
+Use CORS in your Express app:
+javascript
+Copy code
+const cors = require('cors');
+app.use(cors()); // Enable CORS for all routes
+You can also configure CORS options to allow specific domains or HTTP methods.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Abhay Bharati:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1. How can you implement authentication in an Express application?
+Authentication can be implemented using several methods, such as:
+Sessions: Use express-session to create a session for each user. Store user data in the session after successful login.
+JWT (JSON Web Tokens): Use the jsonwebtoken package to generate tokens upon successful login. Send the token to the client, which must include it in the Authorization header for subsequent requests.
+OAuth: Integrate with external providers like Google, Facebook, etc., using libraries like passport.js for easy implementation of various strategies.
+2. What are the best practices for structuring an Express application?
+MVC Structure: Organize your application into Models, Views, and Controllers.
+Models: Define your data schema and interact with the database.
+Controllers: Handle request logic, responding to client requests.
+Routes: Define routes and link them to the appropriate controllers.
+Middleware: Keep middleware logic modular and reusable.
+Environment Variables: Use a .env file to manage configuration settings.
+Error Handling: Centralize error handling middleware to manage application errors cleanly.
+Static Files: Serve static files from a dedicated directory.
+3. How do you implement rate limiting in Express?
+Rate limiting can be implemented using the express-rate-limit package. Here’s a simple example:
+javascript
+Copy code
+const rateLimit = require('express-rate-limit');
+const limiter = rateLimit({
+  windowMs: 15 * 60 * 1000, // 15 minutes
+  max: 100 // limit each IP to 100 requests per windowMs
+});
+app.use(limiter); // Apply to all requests
+This middleware will limit the number of requests from a single IP address.
+4. What is the role of the next() function in Express?
+The next() function is used to pass control to the next middleware function in the stack. If you have multiple middleware functions, calling next() allows the next one to execute. If an error occurs, you can pass an error to next(err), which will skip to the error-handling middleware.
+5. How can you integrate a template engine (like Pug or EJS) with Express?
+To integrate a template engine:
+Install the template engine, e.g., npm install pug or npm install ejs.
+Set the view engine in your Express app:
+javascript
+Copy code
+app.set('view engine', 'pug'); // for Pug
+// or
+app.set('view engine', 'ejs'); // for EJS
+Create a views directory, and place your template files there.
+Render views in your routes:
+javascript
+Copy code
+app.get('/', (req, res) =&gt; {
+  res.render('index', { title: 'Home' });
+});
+6. How do you handle file uploads in Express?
+File uploads can be handled using the multer middleware:
+Install Multer: npm install multer.
+Set up Multer in your Express app:
+javascript
+Copy code
+const multer = require('multer');
+const upload = multer({ dest: 'uploads/' }); // specify the directory to store uploaded files
+app.post('/upload', upload.single('file'), (req, res) =&gt; {
+  res.send('File uploaded successfully!');
+});
+This code sets up an endpoint to accept a single file upload.
+7. What is the purpose of using environment variables in an Express app?
+Environment variables are used to manage configuration settings such as API keys, database connection strings, and application secrets without hardcoding them into your application code. This approach enhances security and makes it easier to manage different configurations for development, testing, and production environments. Use the dotenv package to load environment variables from a .env file:
+javascript
+Copy code
+require('dotenv').config();
+const dbConnectionString = process.env.DB_CONNECTION_STRING;
+8. How do you connect an Express application to a database (e.g., MongoDB)?
+To connect to MongoDB using Mongoose:
+Install Mongoose: npm install mongoose.
+Use Mongoose to connect to your database:
+javascript
+Copy code
+const mongoose = require('mongoose');
+mongoose.connect(process.env.DB_CONNECTION_STRING, { useNewUrlParser: true, useUnifiedTopology: true })
+  .then(() =&gt; console.log('MongoDB connected'))
+  .catch(err =&gt; console.error('MongoDB connection error:', err));
+9. What is the significance of promises and async/await in Express?
+Promises and async/await are used for handling asynchronous operations, such as database queries or external API calls, in a more readable way compared to traditional callbacks. With async/await, you can write asynchronous code that looks synchronous:
+javascript
+Copy code
+app.get('/data', async (req, res) =&gt; {
+  try {
+    const data = await fetchDataFromDatabase();
+    res.json(data);
+  } catch (error) {
+    res.status(500).send('Error fetching data');
+  }
+});
+This approach simplifies error handling and improves code readability.
+10. How can you implement a logging mechanism in Express?
+You can implement logging using middleware like morgan:
+Install Morgan: npm install morgan.
+Set up Morgan in your Express app:
+javascript
+Copy code
+const morgan = require('morgan');
+app.use(morgan('combined')); // Logs requests in Apache combined format</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>EEE</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Abhay Bharati:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 What is MongoDB?
 MongoDB is a popular NoSQL database that uses a document-oriented data model. It stores data in flexible, JSON-like documents called BSON (Binary JSON), allowing for rich data types and a dynamic schema. This flexibility makes MongoDB well-suited for applications with varying data structures.
 Why Use MongoDB?
@@ -2652,7 +2904,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="257">
   <si>
     <t>Hoisting</t>
   </si>
@@ -3943,6 +4195,114 @@
   </si>
   <si>
     <t>Additional Interview-Based Concept</t>
+  </si>
+  <si>
+    <t>Core Concept of Express Js</t>
+  </si>
+  <si>
+    <t>Advance Concept of Express Js</t>
+  </si>
+  <si>
+    <t>What is Express.js, and how does it differ from Node.js?</t>
+  </si>
+  <si>
+    <t>How do you set up a basic Express server?</t>
+  </si>
+  <si>
+    <t>What are middleware in Express, and how do they work?</t>
+  </si>
+  <si>
+    <t>How can you handle routing in Express?</t>
+  </si>
+  <si>
+    <t>How do you handle errors in an Express application?</t>
+  </si>
+  <si>
+    <t>What are the different types of HTTP methods supported by Express?</t>
+  </si>
+  <si>
+    <t>How can you serve static files using Express?</t>
+  </si>
+  <si>
+    <t>How do you parse JSON and URL-encoded data in Express?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the purpose of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>app.use()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function?</t>
+    </r>
+  </si>
+  <si>
+    <t>How can you implement CORS in an Express application?</t>
+  </si>
+  <si>
+    <t>How can you implement authentication in an Express application?</t>
+  </si>
+  <si>
+    <t>What are the best practices for structuring an Express application?</t>
+  </si>
+  <si>
+    <t>How do you implement rate limiting in Express?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What is the role of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>next()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function in Express?</t>
+    </r>
+  </si>
+  <si>
+    <t>How can you integrate a template engine (like Pug or EJS) with Express?</t>
+  </si>
+  <si>
+    <t>How do you handle file uploads in Express?</t>
+  </si>
+  <si>
+    <t>What is the purpose of using environment variables in an Express app?</t>
+  </si>
+  <si>
+    <t>How do you connect an Express application to a database (e.g., MongoDB)?</t>
+  </si>
+  <si>
+    <t>What is the significance of promises and async/await in Express?</t>
+  </si>
+  <si>
+    <t>How can you implement a logging mechanism in Express?</t>
   </si>
 </sst>
 </file>
@@ -4123,7 +4483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4176,6 +4536,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4475,6 +4837,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4726,6 +5091,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4997,10 +5365,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5291,10 +5662,145 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="67.42578125" customWidth="1"/>
+    <col min="2" max="2" width="84.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45">
+      <c r="A2" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="30">
+      <c r="A3" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="30">
+      <c r="A4" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="30.75">
+      <c r="A5" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="45">
+      <c r="A6" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="30">
+      <c r="A7" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="45">
+      <c r="A8" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" ht="45">
+      <c r="A9" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" ht="45">
+      <c r="A10" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="30">
+      <c r="A11" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5315,7 +5821,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45">
+    <row r="2" spans="1:3" ht="30">
       <c r="A2" s="21" t="s">
         <v>162</v>
       </c>
@@ -5337,7 +5843,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="30">
       <c r="A4" s="21" t="s">
         <v>164</v>
       </c>
@@ -5403,7 +5909,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="21" t="s">
         <v>170</v>
       </c>
@@ -5432,12 +5938,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>